<commit_message>
fixed error with multigrid and changed the exit point to just behind the register
</commit_message>
<xml_diff>
--- a/data/albert_excel_test_backup.xlsx
+++ b/data/albert_excel_test_backup.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coen_\Documents\Uva\Agent-based\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{41D21227-DC80-42FD-BDEF-CE9F5C660DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2989BF33-5BCE-4F54-9435-5741EEBB1AF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D53A71B6-3424-4C0C-AE5E-AAFFFD8E2691}"/>
   </bookViews>
@@ -30,6 +30,10 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -175,7 +179,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +324,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -333,7 +343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -377,6 +387,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -698,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38C9D108-BD5D-49AB-8603-E6FF47D0FA07}">
   <dimension ref="A1:CJ61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T48" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="CI79" sqref="CI79"/>
+    <sheetView tabSelected="1" topLeftCell="T13" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="CC25" sqref="CC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="1.88671875" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4402,47 +4413,47 @@
       <c r="BP14" s="30">
         <v>130</v>
       </c>
-      <c r="BQ14" s="30">
-        <v>130</v>
+      <c r="BQ14" s="43">
+        <v>99</v>
       </c>
       <c r="BR14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD14" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE14" s="20">
         <v>99</v>
@@ -4668,47 +4679,47 @@
       <c r="BP15" s="30">
         <v>130</v>
       </c>
-      <c r="BQ15" s="30">
-        <v>130</v>
+      <c r="BQ15" s="43">
+        <v>99</v>
       </c>
       <c r="BR15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD15" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE15" s="20">
         <v>99</v>
@@ -4934,47 +4945,47 @@
       <c r="BP16" s="30">
         <v>130</v>
       </c>
-      <c r="BQ16" s="30">
-        <v>130</v>
+      <c r="BQ16" s="43">
+        <v>99</v>
       </c>
       <c r="BR16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD16" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE16" s="20">
         <v>99</v>
@@ -5200,47 +5211,47 @@
       <c r="BP17" s="30">
         <v>130</v>
       </c>
-      <c r="BQ17" s="30">
-        <v>130</v>
+      <c r="BQ17" s="43">
+        <v>99</v>
       </c>
       <c r="BR17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD17" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE17" s="20">
         <v>99</v>
@@ -5469,44 +5480,44 @@
       <c r="BQ18" s="23">
         <v>100</v>
       </c>
-      <c r="BR18" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS18" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT18" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU18" s="23">
+      <c r="BR18" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS18" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT18" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU18" s="30">
         <v>100</v>
       </c>
       <c r="BV18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD18" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE18" s="20">
         <v>99</v>
@@ -5735,44 +5746,44 @@
       <c r="BQ19" s="23">
         <v>100</v>
       </c>
-      <c r="BR19" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS19" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT19" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU19" s="23">
+      <c r="BR19" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS19" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT19" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU19" s="30">
         <v>100</v>
       </c>
       <c r="BV19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD19" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE19" s="20">
         <v>99</v>
@@ -6001,44 +6012,44 @@
       <c r="BQ20" s="23">
         <v>100</v>
       </c>
-      <c r="BR20" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS20" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT20" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU20" s="23">
+      <c r="BR20" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS20" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT20" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU20" s="30">
         <v>100</v>
       </c>
       <c r="BV20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD20" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE20" s="20">
         <v>99</v>
@@ -6267,44 +6278,44 @@
       <c r="BQ21" s="23">
         <v>100</v>
       </c>
-      <c r="BR21" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS21" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT21" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU21" s="23">
+      <c r="BR21" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS21" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT21" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU21" s="30">
         <v>100</v>
       </c>
       <c r="BV21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD21" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE21" s="20">
         <v>99</v>
@@ -6530,47 +6541,47 @@
       <c r="BP22" s="30">
         <v>130</v>
       </c>
-      <c r="BQ22" s="30">
-        <v>130</v>
+      <c r="BQ22" s="43">
+        <v>99</v>
       </c>
       <c r="BR22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD22" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE22" s="20">
         <v>99</v>
@@ -6796,47 +6807,47 @@
       <c r="BP23" s="30">
         <v>130</v>
       </c>
-      <c r="BQ23" s="30">
-        <v>130</v>
+      <c r="BQ23" s="43">
+        <v>99</v>
       </c>
       <c r="BR23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD23" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE23" s="20">
         <v>99</v>
@@ -7062,47 +7073,47 @@
       <c r="BP24" s="30">
         <v>130</v>
       </c>
-      <c r="BQ24" s="30">
-        <v>130</v>
+      <c r="BQ24" s="43">
+        <v>99</v>
       </c>
       <c r="BR24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD24" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE24" s="20">
         <v>99</v>
@@ -7328,47 +7339,47 @@
       <c r="BP25" s="30">
         <v>130</v>
       </c>
-      <c r="BQ25" s="30">
-        <v>130</v>
+      <c r="BQ25" s="43">
+        <v>99</v>
       </c>
       <c r="BR25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD25" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE25" s="20">
         <v>99</v>
@@ -7597,44 +7608,44 @@
       <c r="BQ26" s="23">
         <v>100</v>
       </c>
-      <c r="BR26" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS26" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT26" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU26" s="23">
+      <c r="BR26" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS26" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT26" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU26" s="30">
         <v>100</v>
       </c>
       <c r="BV26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD26" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE26" s="20">
         <v>99</v>
@@ -7863,44 +7874,44 @@
       <c r="BQ27" s="23">
         <v>100</v>
       </c>
-      <c r="BR27" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS27" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT27" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU27" s="23">
+      <c r="BR27" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS27" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT27" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU27" s="30">
         <v>100</v>
       </c>
       <c r="BV27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD27" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE27" s="20">
         <v>99</v>
@@ -8129,44 +8140,44 @@
       <c r="BQ28" s="23">
         <v>100</v>
       </c>
-      <c r="BR28" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS28" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT28" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU28" s="23">
+      <c r="BR28" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS28" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT28" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU28" s="30">
         <v>100</v>
       </c>
       <c r="BV28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD28" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE28" s="20">
         <v>99</v>
@@ -8395,44 +8406,44 @@
       <c r="BQ29" s="23">
         <v>100</v>
       </c>
-      <c r="BR29" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS29" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT29" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU29" s="23">
+      <c r="BR29" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS29" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT29" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU29" s="30">
         <v>100</v>
       </c>
       <c r="BV29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD29" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE29" s="20">
         <v>99</v>
@@ -8658,46 +8669,46 @@
       <c r="BP30" s="30">
         <v>130</v>
       </c>
-      <c r="BQ30" s="30">
-        <v>130</v>
+      <c r="BQ30" s="43">
+        <v>99</v>
       </c>
       <c r="BR30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX30" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY30" s="30">
-        <v>130</v>
-      </c>
-      <c r="BZ30" s="17">
-        <v>30</v>
-      </c>
-      <c r="CA30" s="17">
-        <v>30</v>
-      </c>
-      <c r="CB30" s="17">
-        <v>30</v>
-      </c>
-      <c r="CC30" s="20">
-        <v>100</v>
-      </c>
-      <c r="CD30" s="20">
+        <v>100</v>
+      </c>
+      <c r="BZ30" s="30">
+        <v>100</v>
+      </c>
+      <c r="CA30" s="30">
+        <v>100</v>
+      </c>
+      <c r="CB30" s="30">
+        <v>100</v>
+      </c>
+      <c r="CC30" s="30">
+        <v>100</v>
+      </c>
+      <c r="CD30" s="30">
         <v>100</v>
       </c>
       <c r="CE30" s="20">
@@ -8924,46 +8935,46 @@
       <c r="BP31" s="30">
         <v>130</v>
       </c>
-      <c r="BQ31" s="30">
-        <v>130</v>
+      <c r="BQ31" s="43">
+        <v>99</v>
       </c>
       <c r="BR31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX31" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY31" s="30">
-        <v>130</v>
-      </c>
-      <c r="BZ31" s="17">
-        <v>30</v>
-      </c>
-      <c r="CA31" s="20">
-        <v>100</v>
-      </c>
-      <c r="CB31" s="20">
-        <v>100</v>
-      </c>
-      <c r="CC31" s="20">
-        <v>100</v>
-      </c>
-      <c r="CD31" s="20">
+        <v>100</v>
+      </c>
+      <c r="BZ31" s="30">
+        <v>100</v>
+      </c>
+      <c r="CA31" s="30">
+        <v>100</v>
+      </c>
+      <c r="CB31" s="30">
+        <v>100</v>
+      </c>
+      <c r="CC31" s="30">
+        <v>100</v>
+      </c>
+      <c r="CD31" s="30">
         <v>100</v>
       </c>
       <c r="CE31" s="20">
@@ -9190,46 +9201,46 @@
       <c r="BP32" s="30">
         <v>130</v>
       </c>
-      <c r="BQ32" s="30">
-        <v>130</v>
+      <c r="BQ32" s="43">
+        <v>99</v>
       </c>
       <c r="BR32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX32" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY32" s="30">
-        <v>130</v>
-      </c>
-      <c r="BZ32" s="17">
-        <v>30</v>
-      </c>
-      <c r="CA32" s="17">
-        <v>30</v>
-      </c>
-      <c r="CB32" s="17">
-        <v>30</v>
-      </c>
-      <c r="CC32" s="20">
-        <v>100</v>
-      </c>
-      <c r="CD32" s="20">
+        <v>100</v>
+      </c>
+      <c r="BZ32" s="30">
+        <v>100</v>
+      </c>
+      <c r="CA32" s="30">
+        <v>100</v>
+      </c>
+      <c r="CB32" s="30">
+        <v>100</v>
+      </c>
+      <c r="CC32" s="30">
+        <v>100</v>
+      </c>
+      <c r="CD32" s="30">
         <v>100</v>
       </c>
       <c r="CE32" s="20">
@@ -9456,47 +9467,47 @@
       <c r="BP33" s="30">
         <v>130</v>
       </c>
-      <c r="BQ33" s="30">
-        <v>130</v>
+      <c r="BQ33" s="43">
+        <v>99</v>
       </c>
       <c r="BR33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD33" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE33" s="20">
         <v>99</v>
@@ -9725,44 +9736,44 @@
       <c r="BQ34" s="23">
         <v>100</v>
       </c>
-      <c r="BR34" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS34" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT34" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU34" s="23">
+      <c r="BR34" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS34" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT34" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU34" s="30">
         <v>100</v>
       </c>
       <c r="BV34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD34" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE34" s="20">
         <v>99</v>
@@ -9991,44 +10002,44 @@
       <c r="BQ35" s="23">
         <v>100</v>
       </c>
-      <c r="BR35" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS35" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT35" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU35" s="23">
+      <c r="BR35" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS35" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT35" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU35" s="30">
         <v>100</v>
       </c>
       <c r="BV35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD35" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE35" s="20">
         <v>99</v>
@@ -10257,44 +10268,44 @@
       <c r="BQ36" s="23">
         <v>100</v>
       </c>
-      <c r="BR36" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS36" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT36" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU36" s="23">
+      <c r="BR36" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS36" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT36" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU36" s="30">
         <v>100</v>
       </c>
       <c r="BV36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD36" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE36" s="20">
         <v>99</v>
@@ -10523,44 +10534,44 @@
       <c r="BQ37" s="23">
         <v>100</v>
       </c>
-      <c r="BR37" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS37" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT37" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU37" s="23">
+      <c r="BR37" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS37" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT37" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU37" s="30">
         <v>100</v>
       </c>
       <c r="BV37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD37" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE37" s="20">
         <v>99</v>
@@ -10789,44 +10800,44 @@
       <c r="BQ38" s="23">
         <v>100</v>
       </c>
-      <c r="BR38" s="23">
-        <v>100</v>
-      </c>
-      <c r="BS38" s="23">
-        <v>100</v>
-      </c>
-      <c r="BT38" s="23">
-        <v>100</v>
-      </c>
-      <c r="BU38" s="23">
+      <c r="BR38" s="30">
+        <v>100</v>
+      </c>
+      <c r="BS38" s="30">
+        <v>100</v>
+      </c>
+      <c r="BT38" s="30">
+        <v>100</v>
+      </c>
+      <c r="BU38" s="30">
         <v>100</v>
       </c>
       <c r="BV38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD38" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE38" s="20">
         <v>99</v>
@@ -11052,47 +11063,47 @@
       <c r="BP39" s="30">
         <v>130</v>
       </c>
-      <c r="BQ39" s="30">
-        <v>130</v>
+      <c r="BQ39" s="43">
+        <v>99</v>
       </c>
       <c r="BR39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD39" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE39" s="20">
         <v>99</v>
@@ -11318,47 +11329,47 @@
       <c r="BP40" s="30">
         <v>130</v>
       </c>
-      <c r="BQ40" s="30">
-        <v>130</v>
+      <c r="BQ40" s="43">
+        <v>99</v>
       </c>
       <c r="BR40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BS40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BT40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BU40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BV40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BW40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BX40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BY40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="BZ40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CA40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CB40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CC40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CD40" s="30">
-        <v>130</v>
+        <v>100</v>
       </c>
       <c r="CE40" s="20">
         <v>99</v>

</xml_diff>